<commit_message>
updating structure and clarifying expectations
</commit_message>
<xml_diff>
--- a/Test Cases/Example Test Cases.xlsx
+++ b/Test Cases/Example Test Cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philmcneely/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philmcneely/git/Class12CapstoneExample/Test Cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -996,17 +996,20 @@
     <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1016,15 +1019,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="17" xfId="42" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1053,20 +1047,26 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1417,120 +1417,120 @@
   <dimension ref="A1:K749"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.3984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.3984375" style="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="5"/>
+    <col min="10" max="10" width="10.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.796875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="33" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="25"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="23"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="33" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="28"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="26"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="36" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="28"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="26"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="28"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="36" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="28"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="36" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="31"/>
-    </row>
-    <row r="9" spans="2:11" ht="43" x14ac:dyDescent="0.2">
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
+    </row>
+    <row r="9" spans="2:11" ht="57" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>7</v>
       </c>
@@ -1563,16 +1563,16 @@
       </c>
     </row>
     <row r="10" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="33" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="10" t="s">
@@ -1581,56 +1581,56 @@
       <c r="G10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="16"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="36"/>
     </row>
     <row r="11" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="18"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="21"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="34"/>
       <c r="F11" s="10" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="16"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="36"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="19"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="22"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="10" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="10"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="16"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="36"/>
     </row>
     <row r="13" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="33" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="10" t="s">
@@ -1639,54 +1639,54 @@
       <c r="G13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="16"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="36"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="18"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="21"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="34"/>
       <c r="F14" s="10" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="16"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="36"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="19"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="22"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="35"/>
       <c r="F15" s="10" t="s">
         <v>15</v>
       </c>
       <c r="G15" s="10"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="16"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="36"/>
     </row>
     <row r="16" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="33" t="s">
         <v>24</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -1695,54 +1695,54 @@
       <c r="G16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="16"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="36"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="18"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="21"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="34"/>
       <c r="F17" s="10" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="16"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="36"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="19"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="22"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="35"/>
       <c r="F18" s="10" t="s">
         <v>15</v>
       </c>
       <c r="G18" s="10"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="16"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="36"/>
     </row>
     <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="33" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="10" t="s">
@@ -1751,45 +1751,47 @@
       <c r="G19" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="16"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="36"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="18"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="21"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="34"/>
       <c r="F20" s="10" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="16"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="36"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="19"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="22"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="35"/>
       <c r="F21" s="10" t="s">
         <v>15</v>
       </c>
       <c r="G21" s="10"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="16"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="36"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="3"/>
+      <c r="B22" s="3">
+        <v>5</v>
+      </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -1802,7 +1804,9 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2">
+        <v>6</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1815,7 +1819,9 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2">
+        <v>7</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1828,7 +1834,9 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2">
+        <v>8</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1841,7 +1849,9 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2">
+        <v>9</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1853,7 +1863,9 @@
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="6"/>
+      <c r="B27" s="6">
+        <v>10</v>
+      </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -10530,13 +10542,28 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="J19:J21"/>
+    <mergeCell ref="K19:K21"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="C16:C18"/>
     <mergeCell ref="B16:B18"/>
     <mergeCell ref="H2:K7"/>
     <mergeCell ref="B10:B12"/>
@@ -10553,28 +10580,13 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="J19:J21"/>
-    <mergeCell ref="K19:K21"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="J10:J12"/>
-    <mergeCell ref="J13:J15"/>
-    <mergeCell ref="J16:J18"/>
-    <mergeCell ref="K10:K12"/>
-    <mergeCell ref="K13:K15"/>
-    <mergeCell ref="K16:K18"/>
-    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>